<commit_message>
Test Plan - updated
</commit_message>
<xml_diff>
--- a/Test Plan/Test Plan.xlsx
+++ b/Test Plan/Test Plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t xml:space="preserve">TEST PLAN FOR SauceDemo </t>
   </si>
@@ -67,82 +67,85 @@
     <t>Account lock/unlock, password reset, multi-factor authentication</t>
   </si>
   <si>
+    <t>Manual + Automation Testing (Selenium + TestNG)</t>
+  </si>
+  <si>
+    <t>Pass if all user types accept or reject with correct messages and UI behavior</t>
+  </si>
+  <si>
+    <t>Testing paused if login form or essential fields are missing</t>
+  </si>
+  <si>
+    <t>Windows 10/11, Chrome, Firefox, Edge</t>
+  </si>
+  <si>
+    <t>Hemant Bhase</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>No risk</t>
+  </si>
+  <si>
+    <t>Vaishali Sonanis</t>
+  </si>
+  <si>
+    <t>- Locked out user error</t>
+  </si>
+  <si>
+    <t>- Problem user login</t>
+  </si>
+  <si>
+    <t>- Performance glitch user login</t>
+  </si>
+  <si>
+    <t>- Error user login</t>
+  </si>
+  <si>
+    <t>- Visual user login</t>
+  </si>
+  <si>
+    <t>- Blank username field</t>
+  </si>
+  <si>
+    <t>- Blank password field</t>
+  </si>
+  <si>
+    <t>- Valid/Invalid password error message</t>
+  </si>
+  <si>
+    <t>- Password masking</t>
+  </si>
+  <si>
+    <t>- Login button enabled/disabled states</t>
+  </si>
+  <si>
+    <t>Inventory Page</t>
+  </si>
+  <si>
+    <t>Product tiles: Image, Name, Price, Description, Add to Cart Button</t>
+  </si>
+  <si>
+    <t>Pagination, User Reviews</t>
+  </si>
+  <si>
+    <t>Pass if all product elements load &amp; interact correctly</t>
+  </si>
+  <si>
+    <t>Testing paused if page fails to load or elements missing</t>
+  </si>
+  <si>
+    <t>Cart Page</t>
+  </si>
+  <si>
+    <t>- Product details (name, price, description) shown</t>
+  </si>
+  <si>
+    <t>Coupon entry, shipping options, bulk updates</t>
+  </si>
+  <si>
     <t>Automation Testing (Selenium + TestNG)</t>
-  </si>
-  <si>
-    <t>Pass if all user types accept or reject with correct messages and UI behavior</t>
-  </si>
-  <si>
-    <t>Testing paused if login form or essential fields are missing</t>
-  </si>
-  <si>
-    <t>Windows 10/11, Chrome, Firefox, Edge</t>
-  </si>
-  <si>
-    <t>Hemant Bhase</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>No risk</t>
-  </si>
-  <si>
-    <t>Vaishali Sonanis</t>
-  </si>
-  <si>
-    <t>- Locked out user error</t>
-  </si>
-  <si>
-    <t>- Problem user login</t>
-  </si>
-  <si>
-    <t>- Performance glitch user login</t>
-  </si>
-  <si>
-    <t>- Error user login</t>
-  </si>
-  <si>
-    <t>- Visual user login</t>
-  </si>
-  <si>
-    <t>- Blank username field</t>
-  </si>
-  <si>
-    <t>- Blank password field</t>
-  </si>
-  <si>
-    <t>- Valid/Invalid password error message</t>
-  </si>
-  <si>
-    <t>- Password masking</t>
-  </si>
-  <si>
-    <t>- Login button enabled/disabled states</t>
-  </si>
-  <si>
-    <t>Inventory Page</t>
-  </si>
-  <si>
-    <t>Product tiles: Image, Name, Price, Description, Add to Cart Button</t>
-  </si>
-  <si>
-    <t>Pagination, User Reviews</t>
-  </si>
-  <si>
-    <t>Pass if all product elements load &amp; interact correctly</t>
-  </si>
-  <si>
-    <t>Testing paused if page fails to load or elements missing</t>
-  </si>
-  <si>
-    <t>Cart Page</t>
-  </si>
-  <si>
-    <t>- Product details (name, price, description) shown</t>
-  </si>
-  <si>
-    <t>Coupon entry, shipping options, bulk updates</t>
   </si>
   <si>
     <t>Pass if cart shows correct products, allows quantity and removal, and 'Checkout'/'Continue Shopping' work as intended</t>
@@ -993,13 +996,13 @@
         <v>42</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>20</v>
@@ -1021,7 +1024,7 @@
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
@@ -1037,7 +1040,7 @@
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
@@ -1053,7 +1056,7 @@
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
@@ -1069,7 +1072,7 @@
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
@@ -1085,7 +1088,7 @@
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>

</xml_diff>